<commit_message>
add Docker and schedule.xls docs
</commit_message>
<xml_diff>
--- a/Docs/Schedule.xlsx
+++ b/Docs/Schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
   <si>
     <t>Introduction to DevOps - Introduction to the definition, value, history, building blocks. Introduction to how Agile software development process applies to DevOps. The importance of integrating source control in DevOps. How automation is applied to DevOps</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>https://zoom.us/recording/share/mlraogdOKDrn2rl-9kk6Of9anXE-mYdujPoqoNEyMYGwIumekTziMw?startTime=1561654677000</t>
+  </si>
+  <si>
+    <t>https://zoom.us/recording/share/0cB7bdNC22KwtqFfrSVZ00CHZ5x5LZZ-Yna67qWQYMqwIumekTziMw?startTime=1561741589000</t>
   </si>
 </sst>
 </file>
@@ -306,10 +309,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -593,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,10 +635,10 @@
       <c r="C2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7">
         <v>43643</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -649,10 +652,10 @@
       <c r="C3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="7">
         <v>43643</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -666,10 +669,10 @@
       <c r="C4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <v>43643</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -683,10 +686,10 @@
       <c r="C5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>43642</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>62</v>
       </c>
     </row>
@@ -700,10 +703,10 @@
       <c r="C6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <v>43641</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -750,10 +753,12 @@
       <c r="C10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="7">
         <v>43644</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -839,8 +844,12 @@
       <c r="B18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="7">
+        <v>43648</v>
+      </c>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -971,8 +980,9 @@
     <hyperlink ref="E2" r:id="rId3"/>
     <hyperlink ref="E3" r:id="rId4"/>
     <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="E10" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>